<commit_message>
update drawing recognition analyses scripts
updat
</commit_message>
<xml_diff>
--- a/analysis/museumstation/1_get_sketches/all_cdm_items.xlsx
+++ b/analysis/museumstation/1_get_sketches/all_cdm_items.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brialong/Documents/GitHub/kiddraw/analysis/museumstation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brialong/Documents/GitHub/kiddraw/analysis/museumstation/1_get_sketches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43F905B-46EB-3540-BD08-B4BF87619A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D44BDF-8314-384C-9C9B-A08416C972E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="820" windowWidth="28040" windowHeight="17040" xr2:uid="{09828A9D-5624-9A45-82AB-F087D8BCCF48}"/>
+    <workbookView xWindow="16560" yWindow="760" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{09828A9D-5624-9A45-82AB-F087D8BCCF48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="notes" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="notes" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$39</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="127">
   <si>
     <t>a bear</t>
   </si>
@@ -266,6 +268,156 @@
   </si>
   <si>
     <t>cdm_run_v3 -- has 23 categories; was not changing run number with each new set of categories; car is duplicated across two sessions at the museumstation.</t>
+  </si>
+  <si>
+    <t>1                         airplane</t>
+  </si>
+  <si>
+    <t>2                            apple</t>
+  </si>
+  <si>
+    <t>3                             bear</t>
+  </si>
+  <si>
+    <t>4                              bed</t>
+  </si>
+  <si>
+    <t>5                              bee</t>
+  </si>
+  <si>
+    <t>6                             bike</t>
+  </si>
+  <si>
+    <t>7                             bird</t>
+  </si>
+  <si>
+    <t>8                             boat</t>
+  </si>
+  <si>
+    <t>9                             book</t>
+  </si>
+  <si>
+    <t>10                          bottle</t>
+  </si>
+  <si>
+    <t>11                            bowl</t>
+  </si>
+  <si>
+    <t>12                          cactus</t>
+  </si>
+  <si>
+    <t>13                           camel</t>
+  </si>
+  <si>
+    <t>14                             car</t>
+  </si>
+  <si>
+    <t>15                             cat</t>
+  </si>
+  <si>
+    <t>16                           chair</t>
+  </si>
+  <si>
+    <t>17                           clock</t>
+  </si>
+  <si>
+    <t>18                           couch</t>
+  </si>
+  <si>
+    <t>19                             cow</t>
+  </si>
+  <si>
+    <t>20                             cup</t>
+  </si>
+  <si>
+    <t>21                             dog</t>
+  </si>
+  <si>
+    <t>22                        elephant</t>
+  </si>
+  <si>
+    <t>23                            face</t>
+  </si>
+  <si>
+    <t>24                            fish</t>
+  </si>
+  <si>
+    <t>25                            frog</t>
+  </si>
+  <si>
+    <t>26                            hand</t>
+  </si>
+  <si>
+    <t>27                             hat</t>
+  </si>
+  <si>
+    <t>28                           horse</t>
+  </si>
+  <si>
+    <t>29                           house</t>
+  </si>
+  <si>
+    <t>30                       ice.cream</t>
+  </si>
+  <si>
+    <t>31                             key</t>
+  </si>
+  <si>
+    <t>32                            lamp</t>
+  </si>
+  <si>
+    <t>33                        mushroom</t>
+  </si>
+  <si>
+    <t>34                         octopus</t>
+  </si>
+  <si>
+    <t>35                          person</t>
+  </si>
+  <si>
+    <t>36                           phone</t>
+  </si>
+  <si>
+    <t>37                           piano</t>
+  </si>
+  <si>
+    <t>38                          rabbit</t>
+  </si>
+  <si>
+    <t>39                        scissors</t>
+  </si>
+  <si>
+    <t>40                           sheep</t>
+  </si>
+  <si>
+    <t>41                           snail</t>
+  </si>
+  <si>
+    <t>42                          spider</t>
+  </si>
+  <si>
+    <t>43                           tiger</t>
+  </si>
+  <si>
+    <t>44                           train</t>
+  </si>
+  <si>
+    <t>45                            tree</t>
+  </si>
+  <si>
+    <t>46                              TV</t>
+  </si>
+  <si>
+    <t>47                           watch</t>
+  </si>
+  <si>
+    <t>48                           whale</t>
+  </si>
+  <si>
+    <t>animacy</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -653,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB08DDAD-1E56-584A-A373-8F3BF63C018F}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1660,6 +1812,921 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691AD284-1034-A749-B27C-DC5606D173C0}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC2A66C-B302-AB4B-B3BC-A4681E43BD8B}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24E1EE8-8E77-9940-AF63-3852A2CAABFB}">
   <dimension ref="B4"/>
   <sheetViews>

</xml_diff>